<commit_message>
[dev] update source data.
</commit_message>
<xml_diff>
--- a/source/games.xlsx
+++ b/source/games.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\OneDrive\$Document\@个人\#游戏\#Pokemon\source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{054A73F5-2E57-4E5F-902F-B2B5A1348439}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="8_{054A73F5-2E57-4E5F-902F-B2B5A1348439}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C263A482-B0D5-4FF7-A5E8-533F9CF4DEF5}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{EC55E8A8-14CC-4AC4-AABB-E09B965E3B38}"/>
   </bookViews>
@@ -33,18 +33,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="98">
   <si>
-    <t>chs</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>eng</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>jpn</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>gen</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -329,6 +317,18 @@
   </si>
   <si>
     <t>シールド</t>
+  </si>
+  <si>
+    <t>name_chs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>name_eng</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>name_jpn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -695,39 +695,38 @@
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="15.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -735,13 +734,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -749,13 +748,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -763,13 +762,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -777,13 +776,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -791,13 +790,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D7">
         <v>2</v>
@@ -805,13 +804,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D8">
         <v>2</v>
@@ -819,13 +818,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C9" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D9">
         <v>3</v>
@@ -833,13 +832,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C10" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D10">
         <v>3</v>
@@ -847,13 +846,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C11" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D11">
         <v>3</v>
@@ -861,13 +860,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C12" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D12">
         <v>3</v>
@@ -875,13 +874,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C13" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D13">
         <v>3</v>
@@ -889,13 +888,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C14" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D14">
         <v>4</v>
@@ -903,13 +902,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C15" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D15">
         <v>4</v>
@@ -917,13 +916,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C16" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D16">
         <v>4</v>
@@ -931,13 +930,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C17" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D17">
         <v>4</v>
@@ -945,13 +944,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C18" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D18">
         <v>4</v>
@@ -959,13 +958,13 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C19" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D19">
         <v>5</v>
@@ -973,13 +972,13 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C20" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D20">
         <v>5</v>
@@ -987,13 +986,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C21" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D21">
         <v>5</v>
@@ -1001,13 +1000,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C22" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D22">
         <v>5</v>
@@ -1015,13 +1014,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D23">
         <v>6</v>
@@ -1029,13 +1028,13 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D24">
         <v>6</v>
@@ -1043,13 +1042,13 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C25" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D25">
         <v>6</v>
@@ -1057,13 +1056,13 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C26" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D26">
         <v>6</v>
@@ -1071,13 +1070,13 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C27" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D27">
         <v>7</v>
@@ -1085,13 +1084,13 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C28" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D28">
         <v>7</v>
@@ -1099,13 +1098,13 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C29" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D29">
         <v>7</v>
@@ -1113,13 +1112,13 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C30" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D30">
         <v>7</v>
@@ -1127,13 +1126,13 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B31" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C31" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D31">
         <v>7</v>
@@ -1141,13 +1140,13 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B32" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C32" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D32">
         <v>7</v>
@@ -1155,13 +1154,13 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B33" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C33" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D33">
         <v>8</v>
@@ -1169,13 +1168,13 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B34" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C34" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D34">
         <v>8</v>

</xml_diff>